<commit_message>
Excel templating completed for writing XLSX files
</commit_message>
<xml_diff>
--- a/src/test/resources/xlsx/basicXlsxTemplate.xlsx
+++ b/src/test/resources/xlsx/basicXlsxTemplate.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet {{stringName}} ABC" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Jebt supports single properties.</t>
   </si>
@@ -29,7 +29,19 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Even with Text formatting: Some bold </t>
+      <t>Even with Text formatting: Some bold {{stringName}}! But only the cell font will be preserved. Any</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> text-section</t>
     </r>
     <r>
       <rPr>
@@ -40,25 +52,67 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>{{stringName}}</t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <u/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">! (as long as the token is using a single Style). </t>
-    </r>
+      <t>specific</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>formatting</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> will be discarded.</t>
+    </r>
+  </si>
+  <si>
+    <t>Empty lines are not a problem.</t>
+  </si>
+  <si>
+    <t>{{stringName}} folks, Let Jebt take on the {{stringName}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,6 +122,33 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -95,8 +176,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,37 +484,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F9" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>